<commit_message>
add: content song hindia - topik
</commit_message>
<xml_diff>
--- a/docs/_asset_song_files.xlsx
+++ b/docs/_asset_song_files.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT_ANDROID\FROGOBOX\RELEASE\TEMPLATE-CODE\BaseMusicPlayer\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT_ANDROID\FROGOBOX\RELEASE\Release-Music-Hindia\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E6811A4-E76D-4C76-A5D9-D27CBD048CFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C8820C-8B7D-4C13-A6C1-3A68BCDB354B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE5E1A3E-F3F9-48B6-8650-D84991C3A10B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>songImage (Image Cover)</t>
   </si>
@@ -48,34 +48,85 @@
     <t>albumName (Album Name)</t>
   </si>
   <si>
-    <t>Ascence - About You [NCS Release]</t>
-  </si>
-  <si>
-    <t>NCS - No Copyright Sound</t>
-  </si>
-  <si>
-    <t>No Copyright</t>
-  </si>
-  <si>
-    <t>Cartoon - Why We Lose (feat. Coleman Trapp)</t>
-  </si>
-  <si>
-    <t>Cartoon - On &amp; On (feat. Daniel Levi)</t>
-  </si>
-  <si>
-    <t>ascence_about_you_ncs_release</t>
-  </si>
-  <si>
-    <t>cartoon_on_on_feat_daniel_levi_letra_espanol_subtitulos</t>
-  </si>
-  <si>
-    <t>cartoon_why_we_lose_feat_coleman_trapp_letra_subtitulos_espanol</t>
-  </si>
-  <si>
-    <t>Ascence</t>
-  </si>
-  <si>
-    <t>ic_base_cover_song</t>
+    <t>apapun_yang_terjadi</t>
+  </si>
+  <si>
+    <t>Apapun Yang Terjadi</t>
+  </si>
+  <si>
+    <t>belum_tidur_feat_sal_priadi</t>
+  </si>
+  <si>
+    <t>Belum Tidur (feat. Sal Priadi)</t>
+  </si>
+  <si>
+    <t>Besok Mungkin Kita Sampai</t>
+  </si>
+  <si>
+    <t>Dehidrasi (feat. Petra Sihombing)</t>
+  </si>
+  <si>
+    <t>Evakuasi</t>
+  </si>
+  <si>
+    <t>Evaluasi</t>
+  </si>
+  <si>
+    <t>Jam Makan Siang (feat. Matter Mos)</t>
+  </si>
+  <si>
+    <t>Mata Air (feat. Natasha Udu, Kamga)</t>
+  </si>
+  <si>
+    <t>Membasuh (feat. Rara Sekar)</t>
+  </si>
+  <si>
+    <t>Rumah Ke Rumah</t>
+  </si>
+  <si>
+    <t>Secukupnya</t>
+  </si>
+  <si>
+    <t>Untuk Apa - Untuk Apa</t>
+  </si>
+  <si>
+    <t>Topik</t>
+  </si>
+  <si>
+    <t>Hindia</t>
+  </si>
+  <si>
+    <t>besok_mungkin_kita_sampai</t>
+  </si>
+  <si>
+    <t>dehidrasi</t>
+  </si>
+  <si>
+    <t>evakuasi</t>
+  </si>
+  <si>
+    <t>evaluasi</t>
+  </si>
+  <si>
+    <t>membasuh</t>
+  </si>
+  <si>
+    <t>secukupnya</t>
+  </si>
+  <si>
+    <t>jam_makan_siang</t>
+  </si>
+  <si>
+    <t>mata_air</t>
+  </si>
+  <si>
+    <t>rumah_ke_rumah</t>
+  </si>
+  <si>
+    <t>untuk_apa</t>
+  </si>
+  <si>
+    <t>ic_hindia_cover</t>
   </si>
 </sst>
 </file>
@@ -455,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EBFF7D-D20B-4BFB-AA6D-93FA55356B20}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,53 +540,206 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: SourceCode make simplyfy
</commit_message>
<xml_diff>
--- a/docs/_asset_song_files.xlsx
+++ b/docs/_asset_song_files.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT_ANDROID\TEAM-PLAY\BASE-CODE\BaseMusicPlayerLyric\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECT_ANDROID\FROGOBOX\TEMPLATE-CODE\BaseMusicPlayerLyric\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1520FF2-200F-4BD7-86E8-90EAA40FD2EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAA13A6-8657-400F-BBC0-BFA557EBDFC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE5E1A3E-F3F9-48B6-8650-D84991C3A10B}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>songImage (Image Cover)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>songMusic (Music Title - Filename)</t>
   </si>
@@ -42,12 +39,6 @@
     <t>songName (Music Title)</t>
   </si>
   <si>
-    <t>artistName (Artist Name)</t>
-  </si>
-  <si>
-    <t>albumName (Album Name)</t>
-  </si>
-  <si>
     <t>apapun_yang_terjadi</t>
   </si>
   <si>
@@ -58,15 +49,6 @@
   </si>
   <si>
     <t>Belum Tidur (feat. Sal Priadi)</t>
-  </si>
-  <si>
-    <t>Topik</t>
-  </si>
-  <si>
-    <t>Hindia</t>
-  </si>
-  <si>
-    <t>ic_hindia_cover</t>
   </si>
   <si>
     <t>lyric</t>
@@ -459,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EBFF7D-D20B-4BFB-AA6D-93FA55356B20}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +457,7 @@
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -483,86 +465,59 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>

</xml_diff>